<commit_message>
Avance se piensa en formulas a futuro
</commit_message>
<xml_diff>
--- a/scac/BackEnd/resultado_validaciones_completo.xlsx
+++ b/scac/BackEnd/resultado_validaciones_completo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -689,7 +689,11 @@
           <t>1130643841</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>FABIO ROBINSON MALDONADO ORDOÑEZ</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>FABIO ROBINSON MALDONADO ORDOÑEZ</t>
@@ -697,15 +701,29 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>No especificado en instructores; Diferencia en nombre</t>
+          <t>VERIFICADO</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+      <c r="A7" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>CC</t>
@@ -713,18 +731,22 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>113064384129</t>
+          <t>16698345</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>FABIO ROBINSON MALDONADO ORDOÑEZ</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
+          <t>OMAR URIEL PATIÑO TORRES</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>OMAR URIEL PATIÑO TORRES</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>No especificado en Sofía; Diferencia en nombre</t>
+          <t>VERIFICADO</t>
         </is>
       </c>
     </row>
@@ -754,17 +776,17 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>16698345</t>
+          <t>16739327</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>OMAR URIEL PATIÑO TORRES</t>
+          <t>JOAQUIN BERNARDO LOPEZ PEREA</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>OMAR URIEL PATIÑO TORRES</t>
+          <t>JOAQUIN BERNARDO LOPEZ PEREA</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -799,17 +821,17 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>16739327</t>
+          <t>18464762</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>JOAQUIN BERNARDO LOPEZ PEREA</t>
+          <t>LUIS EDUARDO OLIVEROS RAMIREZ</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>JOAQUIN BERNARDO LOPEZ PEREA</t>
+          <t>LUIS EDUARDO OLIVEROS RAMIREZ</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -844,17 +866,17 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>18464762</t>
+          <t>25018849</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>LUIS EDUARDO OLIVEROS RAMIREZ</t>
+          <t>NORA MARIA BLANDON SERNA</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>LUIS EDUARDO OLIVEROS RAMIREZ</t>
+          <t>NORA MARIA BLANDON SERNA</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -889,17 +911,17 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>25018849</t>
+          <t>31642764</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>NORA MARIA BLANDON SERNA</t>
+          <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>NORA MARIA BLANDON SERNA</t>
+          <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -934,17 +956,17 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>31642764</t>
+          <t>31863992</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
+          <t>ALBA INES ZULETA JARAMILLO</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
+          <t>ALBA INES ZULETA JARAMILLO</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -979,17 +1001,17 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>31863992</t>
+          <t>32731171</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>ALBA INES ZULETA JARAMILLO</t>
+          <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>ALBA INES ZULETA JARAMILLO</t>
+          <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1024,22 +1046,22 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>32731171</t>
+          <t>36380685</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
+          <t>GLORIA YENNY CASTILLO ESPAÑAS</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
+          <t>GLORIA YENNY CASTILLO ESPAÑA</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>VERIFICADO</t>
+          <t>Diferencia en nombre</t>
         </is>
       </c>
     </row>
@@ -1069,17 +1091,17 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>36380685</t>
+          <t>38553002</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>GLORIA YENNY CASTILLO ESPAÑA</t>
+          <t>PAOLA ANDREA CASTILLO ALZATE</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>GLORIA YENNY CASTILLO ESPAÑA</t>
+          <t>PAOLA ANDREA CASTILLO ALZATE</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1114,17 +1136,17 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>38553002</t>
+          <t>42057870</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>PAOLA ANDREA CASTILLO ALZATE</t>
+          <t>MARTHA LUCIA ALZATE GOMEZ</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>PAOLA ANDREA CASTILLO ALZATE</t>
+          <t>MARTHA LUCIA ALZATE GOMEZ</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1159,17 +1181,17 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>42057870</t>
+          <t>66655884</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>MARTHA LUCIA ALZATE GOMEZ</t>
+          <t>MARIA DEL CARMEN CERON BEDOYA</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>MARTHA LUCIA ALZATE GOMEZ</t>
+          <t>MARIA DEL CARMEN CERON BEDOYA</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1179,24 +1201,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
           <t>CC</t>
@@ -1204,22 +1212,18 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>66655884</t>
+          <t>66756576</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>MARIA DEL CARMEN CERON BEDOYA</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>MARIA DEL CARMEN CERON BEDOYA</t>
-        </is>
-      </c>
+          <t>MARTHA ISABEL BENAVIDES ACOSTA</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
-          <t>VERIFICADO</t>
+          <t>No especificado en Sofía; Diferencia en nombre</t>
         </is>
       </c>
     </row>
@@ -1249,65 +1253,20 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>66756576</t>
+          <t>66767235</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>MARTHA ISABEL BENAVIDES ACOSTA</t>
+          <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>MARTHA ISABEL BENAVIDES ACOSTA</t>
+          <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
-        <is>
-          <t>VERIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>66767235</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
         <is>
           <t>VERIFICADO</t>
         </is>

</xml_diff>